<commit_message>
change sql-query and added change column
</commit_message>
<xml_diff>
--- a/job_counts_today.xlsx
+++ b/job_counts_today.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>job_count</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>change</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -451,11 +456,14 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-06-15 13:25:11.986865</t>
+          <t>2024-06-15 20:49:16.736937</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -464,141 +472,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-06-15 13:25:11.988046</t>
+          <t>2024-06-15 20:49:46.269381</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:25:16.455677</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:25:21.464636</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:25:26.461124</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:25:31.456996</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:25:36.458909</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:25:41.462182</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:25:46.459213</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:25:51.459710</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:25:56.461831</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2024-06-15 13:26:01.459310</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
+      <c r="D3" t="n">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create script for starting application
</commit_message>
<xml_diff>
--- a/job_counts_today.xlsx
+++ b/job_counts_today.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,11 +456,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-06-15 20:49:16.736937</t>
+          <t>2024-06-16 10:50:22.225205</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>21399</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -472,14 +472,46 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-06-15 20:49:46.269381</t>
+          <t>2024-06-16 10:50:46.586880</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>21399</v>
       </c>
       <c r="D3" t="n">
-        <v>-2</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2024-06-16 12:49:49.275805</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>21402</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2024-06-16 12:50:15.873938</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>21404</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>